<commit_message>
Adds code to replicate tables 1-6
</commit_message>
<xml_diff>
--- a/data/raw/epu/AUS.xlsx
+++ b/data/raw/epu/AUS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="26">
   <si>
     <t>year</t>
   </si>
@@ -134,7 +134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C263"/>
+  <dimension ref="A1:C260"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -2983,48 +2983,15 @@
         <v>6</v>
       </c>
       <c r="C259" s="0">
-        <v>104.01030731201172</v>
+        <v>106.1590576171875</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>22</v>
-      </c>
-      <c r="B260" s="0">
-        <v>7</v>
-      </c>
-      <c r="C260" s="0">
-        <v>87.194297790527344</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="s">
-        <v>22</v>
-      </c>
-      <c r="B261" s="0">
-        <v>8</v>
-      </c>
-      <c r="C261" s="0">
-        <v>195.44833374023437</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" t="s">
-        <v>22</v>
-      </c>
-      <c r="B262" s="0">
-        <v>9</v>
-      </c>
-      <c r="C262" s="0">
-        <v>139.81910705566406</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" t="s">
         <v>23</v>
       </c>
-      <c r="B263" s="0"/>
-      <c r="C263" s="0"/>
+      <c r="B260" s="0"/>
+      <c r="C260" s="0"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>